<commit_message>
Revert "Update mippy進捗管理表 .xlsx"
This reverts commit 201f0c6bbeb3ef5d9fcf5cbb574e4f656fd99615.
</commit_message>
<xml_diff>
--- a/doc/mippy進捗管理表 .xlsx
+++ b/doc/mippy進捗管理表 .xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C016CD47-E4D3-4102-9DFD-8CA87C1E47BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445C4F36-877C-4FDE-A326-6CEA20C6EF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2607,7 +2607,7 @@
   <dimension ref="A1:AL83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>

</xml_diff>